<commit_message>
removed collector Name auth
</commit_message>
<xml_diff>
--- a/selenium/src/main/java/resources/downloadTotalForm.xlsx
+++ b/selenium/src/main/java/resources/downloadTotalForm.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{82AC1535-6C67-442D-B052-45F3386BDA02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{0DCC0DDF-EE77-4C91-A70F-55DE9FAC69F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{7848483E-65B6-4A6E-A404-203B22FE5CDC}"/>
   </bookViews>
@@ -16,20 +16,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="56">
   <si>
     <t>Payment_Mode</t>
   </si>
@@ -191,6 +183,12 @@
   </si>
   <si>
     <t>DemandDraft</t>
+  </si>
+  <si>
+    <t>PinCode [ yes,no ]</t>
+  </si>
+  <si>
+    <t>AddressState [ yes,no ]</t>
   </si>
 </sst>
 </file>
@@ -554,10 +552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CADA5ABB-7083-47E2-B29F-7442DAD3221C}">
-  <dimension ref="A1:AS14"/>
+  <dimension ref="A1:AU14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,27 +584,29 @@
     <col min="23" max="24" width="14.85546875" customWidth="1"/>
     <col min="25" max="25" width="16.140625" customWidth="1"/>
     <col min="26" max="26" width="15.85546875" customWidth="1"/>
-    <col min="27" max="27" width="9" customWidth="1"/>
-    <col min="28" max="28" width="16.140625" customWidth="1"/>
-    <col min="29" max="29" width="10" customWidth="1"/>
-    <col min="30" max="30" width="17.140625" customWidth="1"/>
-    <col min="31" max="31" width="14.5703125" customWidth="1"/>
-    <col min="32" max="32" width="15.85546875" customWidth="1"/>
-    <col min="33" max="33" width="9.85546875" customWidth="1"/>
-    <col min="34" max="34" width="10.140625" customWidth="1"/>
-    <col min="35" max="35" width="8.85546875" customWidth="1"/>
-    <col min="36" max="36" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="16.7109375" customWidth="1"/>
+    <col min="28" max="28" width="12.5703125" customWidth="1"/>
+    <col min="29" max="29" width="9" customWidth="1"/>
+    <col min="30" max="30" width="16.140625" customWidth="1"/>
+    <col min="31" max="31" width="10" customWidth="1"/>
+    <col min="32" max="32" width="17.140625" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" customWidth="1"/>
+    <col min="34" max="34" width="15.85546875" customWidth="1"/>
+    <col min="35" max="35" width="9.85546875" customWidth="1"/>
+    <col min="36" max="36" width="10.140625" customWidth="1"/>
     <col min="37" max="37" width="8.85546875" customWidth="1"/>
-    <col min="38" max="38" width="9" customWidth="1"/>
-    <col min="39" max="39" width="11" customWidth="1"/>
-    <col min="40" max="40" width="10.28515625" customWidth="1"/>
-    <col min="41" max="41" width="8.7109375" customWidth="1"/>
-    <col min="42" max="42" width="9.42578125" customWidth="1"/>
-    <col min="43" max="43" width="14.85546875" customWidth="1"/>
-    <col min="44" max="45" width="15.7109375" customWidth="1"/>
+    <col min="38" max="38" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="8.85546875" customWidth="1"/>
+    <col min="40" max="40" width="9" customWidth="1"/>
+    <col min="41" max="41" width="11" customWidth="1"/>
+    <col min="42" max="42" width="10.28515625" customWidth="1"/>
+    <col min="43" max="43" width="8.7109375" customWidth="1"/>
+    <col min="44" max="44" width="9.42578125" customWidth="1"/>
+    <col min="45" max="45" width="14.85546875" customWidth="1"/>
+    <col min="46" max="47" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="60" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:47" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -686,64 +686,70 @@
         <v>26</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="AK1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="AL1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AP1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AS1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>47</v>
       </c>
@@ -879,8 +885,14 @@
       <c r="AS2" t="s">
         <v>3</v>
       </c>
+      <c r="AT2" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>46</v>
       </c>
@@ -1016,8 +1028,14 @@
       <c r="AS4" t="s">
         <v>3</v>
       </c>
+      <c r="AT4" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU4" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>49</v>
       </c>
@@ -1153,8 +1171,14 @@
       <c r="AS6" t="s">
         <v>3</v>
       </c>
+      <c r="AT6" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU6" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>53</v>
       </c>
@@ -1290,8 +1314,14 @@
       <c r="AS8" t="s">
         <v>3</v>
       </c>
+      <c r="AT8" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU8" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -1427,8 +1457,14 @@
       <c r="AS10" t="s">
         <v>3</v>
       </c>
+      <c r="AT10" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU10" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>51</v>
       </c>
@@ -1564,13 +1600,19 @@
       <c r="AS12" t="s">
         <v>3</v>
       </c>
+      <c r="AT12" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:47" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>52</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
@@ -1585,10 +1627,10 @@
         <v>3</v>
       </c>
       <c r="G14" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="H14" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="I14" t="s">
         <v>3</v>
@@ -1597,7 +1639,7 @@
         <v>3</v>
       </c>
       <c r="K14" t="s">
-        <v>48</v>
+        <v>3</v>
       </c>
       <c r="L14" t="s">
         <v>3</v>
@@ -1699,6 +1741,12 @@
         <v>3</v>
       </c>
       <c r="AS14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AT14" t="s">
+        <v>3</v>
+      </c>
+      <c r="AU14" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>